<commit_message>
Created Reveneu by Year and Region
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheddyranking\Documents\Collections\Sales Analysis Dashboard with Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA14CAF2-44B1-41A6-89D5-F38A2A259AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F521EBE-1ADF-41B5-8DA8-E1D7ED556F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{07247CAE-FE2B-4A1F-9670-0F301C861A10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{07247CAE-FE2B-4A1F-9670-0F301C861A10}"/>
   </bookViews>
   <sheets>
     <sheet name=" Reveue by Year" sheetId="4" r:id="rId1"/>
@@ -6116,7 +6116,6 @@
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
         <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
@@ -27928,8 +27927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{880C207A-7D91-49E8-A518-78387AA848A3}">
   <dimension ref="A3:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28028,8 +28027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C5EA75-76FD-4685-B9D2-A43B3EC4C825}">
   <dimension ref="A3:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>